<commit_message>
Start Creating Course Table Of Contents
</commit_message>
<xml_diff>
--- a/Course Structure/Topics.xlsx
+++ b/Course Structure/Topics.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D04BBC-D928-46DD-AFE6-01315D088826}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE89419-5B6B-4035-A226-6D342353EBD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Vue.js Playbook" sheetId="1" r:id="rId1"/>
-    <sheet name="Vue Getting Started" sheetId="5" r:id="rId2"/>
-    <sheet name="Vue JS 2 - The Complete Guide" sheetId="2" r:id="rId3"/>
-    <sheet name="Build Web Apps With Vue.js 2&amp; F" sheetId="4" r:id="rId4"/>
+    <sheet name="My Vue Course" sheetId="6" r:id="rId1"/>
+    <sheet name="Vue.js Playbook" sheetId="1" r:id="rId2"/>
+    <sheet name="Vue Getting Started" sheetId="5" r:id="rId3"/>
+    <sheet name="Vue JS 2 - The Complete Guide" sheetId="2" r:id="rId4"/>
+    <sheet name="Build Web Apps With Vue.js 2&amp; F" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="692">
   <si>
     <t>Introducing Vue.js</t>
   </si>
@@ -2087,6 +2088,18 @@
   </si>
   <si>
     <t xml:space="preserve"> Recap of Vuex</t>
+  </si>
+  <si>
+    <t>Beginner - Advanced</t>
+  </si>
+  <si>
+    <t>12, 2019 </t>
+  </si>
+  <si>
+    <t>6h</t>
+  </si>
+  <si>
+    <t>Mohammad Ahmadi</t>
   </si>
 </sst>
 </file>
@@ -2097,7 +2110,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2105,7 +2118,7 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2113,7 +2126,7 @@
       <b/>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2138,7 +2151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2159,6 +2172,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2439,6 +2455,349 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0BBA446-3A88-4C8D-9F03-218296471687}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="38.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="30.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="9">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="4">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1"/>
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>624</v>
+      </c>
+      <c r="B12" t="s">
+        <v>625</v>
+      </c>
+      <c r="C12" t="s">
+        <v>626</v>
+      </c>
+      <c r="D12" t="s">
+        <v>627</v>
+      </c>
+      <c r="E12" t="s">
+        <v>628</v>
+      </c>
+      <c r="F12" t="s">
+        <v>629</v>
+      </c>
+      <c r="G12" t="s">
+        <v>630</v>
+      </c>
+      <c r="H12" t="s">
+        <v>631</v>
+      </c>
+      <c r="I12" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>633</v>
+      </c>
+      <c r="C13" t="s">
+        <v>634</v>
+      </c>
+      <c r="D13" t="s">
+        <v>635</v>
+      </c>
+      <c r="E13" t="s">
+        <v>636</v>
+      </c>
+      <c r="F13" t="s">
+        <v>637</v>
+      </c>
+      <c r="G13" t="s">
+        <v>638</v>
+      </c>
+      <c r="H13" t="s">
+        <v>639</v>
+      </c>
+      <c r="I13" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>641</v>
+      </c>
+      <c r="C14" t="s">
+        <v>642</v>
+      </c>
+      <c r="D14" t="s">
+        <v>643</v>
+      </c>
+      <c r="E14" t="s">
+        <v>644</v>
+      </c>
+      <c r="F14" t="s">
+        <v>645</v>
+      </c>
+      <c r="G14" t="s">
+        <v>646</v>
+      </c>
+      <c r="H14" t="s">
+        <v>647</v>
+      </c>
+      <c r="I14" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>649</v>
+      </c>
+      <c r="C15" t="s">
+        <v>650</v>
+      </c>
+      <c r="D15" t="s">
+        <v>651</v>
+      </c>
+      <c r="E15" t="s">
+        <v>652</v>
+      </c>
+      <c r="F15" t="s">
+        <v>653</v>
+      </c>
+      <c r="G15" t="s">
+        <v>654</v>
+      </c>
+      <c r="H15" t="s">
+        <v>655</v>
+      </c>
+      <c r="I15" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>657</v>
+      </c>
+      <c r="C16" t="s">
+        <v>658</v>
+      </c>
+      <c r="D16" t="s">
+        <v>659</v>
+      </c>
+      <c r="E16" t="s">
+        <v>660</v>
+      </c>
+      <c r="F16" t="s">
+        <v>661</v>
+      </c>
+      <c r="G16" t="s">
+        <v>662</v>
+      </c>
+      <c r="H16" t="s">
+        <v>663</v>
+      </c>
+      <c r="I16" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>665</v>
+      </c>
+      <c r="C17" t="s">
+        <v>666</v>
+      </c>
+      <c r="D17" t="s">
+        <v>667</v>
+      </c>
+      <c r="E17" t="s">
+        <v>668</v>
+      </c>
+      <c r="F17" t="s">
+        <v>669</v>
+      </c>
+      <c r="G17" t="s">
+        <v>670</v>
+      </c>
+      <c r="H17" t="s">
+        <v>671</v>
+      </c>
+      <c r="I17" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>673</v>
+      </c>
+      <c r="C18" t="s">
+        <v>674</v>
+      </c>
+      <c r="E18" t="s">
+        <v>675</v>
+      </c>
+      <c r="F18" t="s">
+        <v>676</v>
+      </c>
+      <c r="H18" t="s">
+        <v>677</v>
+      </c>
+      <c r="I18" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="C19" t="s">
+        <v>679</v>
+      </c>
+      <c r="F19" t="s">
+        <v>680</v>
+      </c>
+      <c r="H19" t="s">
+        <v>681</v>
+      </c>
+      <c r="I19" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="I20" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="I21" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="I22" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="I23" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="I24" t="s">
+        <v>687</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F25"/>
   <sheetViews>
@@ -2446,17 +2805,17 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="33.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
@@ -2464,7 +2823,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>86</v>
       </c>
@@ -2472,7 +2831,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
@@ -2480,7 +2839,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>90</v>
       </c>
@@ -2488,7 +2847,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>92</v>
       </c>
@@ -2496,19 +2855,19 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -2528,7 +2887,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -2548,7 +2907,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -2568,7 +2927,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -2588,7 +2947,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -2608,7 +2967,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -2628,7 +2987,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -2648,7 +3007,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -2668,7 +3027,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -2688,7 +3047,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -2708,7 +3067,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -2728,7 +3087,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -2745,7 +3104,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>22</v>
       </c>
@@ -2759,7 +3118,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
         <v>23</v>
       </c>
@@ -2770,7 +3129,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
         <v>24</v>
       </c>
@@ -2781,7 +3140,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
         <v>25</v>
       </c>
@@ -2792,350 +3151,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>26</v>
       </c>
       <c r="E25" t="s">
         <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I24"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="38.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="30.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="37.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="9" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>615</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>616</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>617</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>618</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>619</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>620</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>621</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>622</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>624</v>
-      </c>
-      <c r="B12" t="s">
-        <v>625</v>
-      </c>
-      <c r="C12" t="s">
-        <v>626</v>
-      </c>
-      <c r="D12" t="s">
-        <v>627</v>
-      </c>
-      <c r="E12" t="s">
-        <v>628</v>
-      </c>
-      <c r="F12" t="s">
-        <v>629</v>
-      </c>
-      <c r="G12" t="s">
-        <v>630</v>
-      </c>
-      <c r="H12" t="s">
-        <v>631</v>
-      </c>
-      <c r="I12" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>633</v>
-      </c>
-      <c r="C13" t="s">
-        <v>634</v>
-      </c>
-      <c r="D13" t="s">
-        <v>635</v>
-      </c>
-      <c r="E13" t="s">
-        <v>636</v>
-      </c>
-      <c r="F13" t="s">
-        <v>637</v>
-      </c>
-      <c r="G13" t="s">
-        <v>638</v>
-      </c>
-      <c r="H13" t="s">
-        <v>639</v>
-      </c>
-      <c r="I13" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>641</v>
-      </c>
-      <c r="C14" t="s">
-        <v>642</v>
-      </c>
-      <c r="D14" t="s">
-        <v>643</v>
-      </c>
-      <c r="E14" t="s">
-        <v>644</v>
-      </c>
-      <c r="F14" t="s">
-        <v>645</v>
-      </c>
-      <c r="G14" t="s">
-        <v>646</v>
-      </c>
-      <c r="H14" t="s">
-        <v>647</v>
-      </c>
-      <c r="I14" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>649</v>
-      </c>
-      <c r="C15" t="s">
-        <v>650</v>
-      </c>
-      <c r="D15" t="s">
-        <v>651</v>
-      </c>
-      <c r="E15" t="s">
-        <v>652</v>
-      </c>
-      <c r="F15" t="s">
-        <v>653</v>
-      </c>
-      <c r="G15" t="s">
-        <v>654</v>
-      </c>
-      <c r="H15" t="s">
-        <v>655</v>
-      </c>
-      <c r="I15" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>657</v>
-      </c>
-      <c r="C16" t="s">
-        <v>658</v>
-      </c>
-      <c r="D16" t="s">
-        <v>659</v>
-      </c>
-      <c r="E16" t="s">
-        <v>660</v>
-      </c>
-      <c r="F16" t="s">
-        <v>661</v>
-      </c>
-      <c r="G16" t="s">
-        <v>662</v>
-      </c>
-      <c r="H16" t="s">
-        <v>663</v>
-      </c>
-      <c r="I16" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>665</v>
-      </c>
-      <c r="C17" t="s">
-        <v>666</v>
-      </c>
-      <c r="D17" t="s">
-        <v>667</v>
-      </c>
-      <c r="E17" t="s">
-        <v>668</v>
-      </c>
-      <c r="F17" t="s">
-        <v>669</v>
-      </c>
-      <c r="G17" t="s">
-        <v>670</v>
-      </c>
-      <c r="H17" t="s">
-        <v>671</v>
-      </c>
-      <c r="I17" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>673</v>
-      </c>
-      <c r="C18" t="s">
-        <v>674</v>
-      </c>
-      <c r="E18" t="s">
-        <v>675</v>
-      </c>
-      <c r="F18" t="s">
-        <v>676</v>
-      </c>
-      <c r="H18" t="s">
-        <v>677</v>
-      </c>
-      <c r="I18" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>679</v>
-      </c>
-      <c r="F19" t="s">
-        <v>680</v>
-      </c>
-      <c r="H19" t="s">
-        <v>681</v>
-      </c>
-      <c r="I19" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="I20" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="I21" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="I22" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="I23" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="I24" t="s">
-        <v>687</v>
       </c>
     </row>
   </sheetData>
@@ -3145,6 +3166,344 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="38.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="30.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="37.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="1"/>
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>620</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>621</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>624</v>
+      </c>
+      <c r="B12" t="s">
+        <v>625</v>
+      </c>
+      <c r="C12" t="s">
+        <v>626</v>
+      </c>
+      <c r="D12" t="s">
+        <v>627</v>
+      </c>
+      <c r="E12" t="s">
+        <v>628</v>
+      </c>
+      <c r="F12" t="s">
+        <v>629</v>
+      </c>
+      <c r="G12" t="s">
+        <v>630</v>
+      </c>
+      <c r="H12" t="s">
+        <v>631</v>
+      </c>
+      <c r="I12" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>633</v>
+      </c>
+      <c r="C13" t="s">
+        <v>634</v>
+      </c>
+      <c r="D13" t="s">
+        <v>635</v>
+      </c>
+      <c r="E13" t="s">
+        <v>636</v>
+      </c>
+      <c r="F13" t="s">
+        <v>637</v>
+      </c>
+      <c r="G13" t="s">
+        <v>638</v>
+      </c>
+      <c r="H13" t="s">
+        <v>639</v>
+      </c>
+      <c r="I13" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>641</v>
+      </c>
+      <c r="C14" t="s">
+        <v>642</v>
+      </c>
+      <c r="D14" t="s">
+        <v>643</v>
+      </c>
+      <c r="E14" t="s">
+        <v>644</v>
+      </c>
+      <c r="F14" t="s">
+        <v>645</v>
+      </c>
+      <c r="G14" t="s">
+        <v>646</v>
+      </c>
+      <c r="H14" t="s">
+        <v>647</v>
+      </c>
+      <c r="I14" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>649</v>
+      </c>
+      <c r="C15" t="s">
+        <v>650</v>
+      </c>
+      <c r="D15" t="s">
+        <v>651</v>
+      </c>
+      <c r="E15" t="s">
+        <v>652</v>
+      </c>
+      <c r="F15" t="s">
+        <v>653</v>
+      </c>
+      <c r="G15" t="s">
+        <v>654</v>
+      </c>
+      <c r="H15" t="s">
+        <v>655</v>
+      </c>
+      <c r="I15" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>657</v>
+      </c>
+      <c r="C16" t="s">
+        <v>658</v>
+      </c>
+      <c r="D16" t="s">
+        <v>659</v>
+      </c>
+      <c r="E16" t="s">
+        <v>660</v>
+      </c>
+      <c r="F16" t="s">
+        <v>661</v>
+      </c>
+      <c r="G16" t="s">
+        <v>662</v>
+      </c>
+      <c r="H16" t="s">
+        <v>663</v>
+      </c>
+      <c r="I16" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>665</v>
+      </c>
+      <c r="C17" t="s">
+        <v>666</v>
+      </c>
+      <c r="D17" t="s">
+        <v>667</v>
+      </c>
+      <c r="E17" t="s">
+        <v>668</v>
+      </c>
+      <c r="F17" t="s">
+        <v>669</v>
+      </c>
+      <c r="G17" t="s">
+        <v>670</v>
+      </c>
+      <c r="H17" t="s">
+        <v>671</v>
+      </c>
+      <c r="I17" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
+        <v>673</v>
+      </c>
+      <c r="C18" t="s">
+        <v>674</v>
+      </c>
+      <c r="E18" t="s">
+        <v>675</v>
+      </c>
+      <c r="F18" t="s">
+        <v>676</v>
+      </c>
+      <c r="H18" t="s">
+        <v>677</v>
+      </c>
+      <c r="I18" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="C19" t="s">
+        <v>679</v>
+      </c>
+      <c r="F19" t="s">
+        <v>680</v>
+      </c>
+      <c r="H19" t="s">
+        <v>681</v>
+      </c>
+      <c r="I19" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="I20" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="I21" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="I22" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="I23" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.45">
+      <c r="I24" t="s">
+        <v>687</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Y71"/>
   <sheetViews>
@@ -3152,37 +3511,37 @@
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="62" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="91.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="49.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="91.265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="83" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="52.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="45.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="58.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="58.3984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="51" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="41.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="62.875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="41.86328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="62.86328125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="57" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="69.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="48.625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="56.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="49.375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="44.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="36.125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="58.75" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="51.625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="53.75" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="47.125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="69.59765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="48.59765625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="56.1328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="49.3984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="44.59765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="36.1328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="58.73046875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="51.59765625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="53.73046875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="47.1328125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="35" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
@@ -3190,7 +3549,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>86</v>
       </c>
@@ -3198,7 +3557,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
@@ -3206,7 +3565,7 @@
         <v>0.90981481481481474</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>97</v>
       </c>
@@ -3214,7 +3573,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>90</v>
       </c>
@@ -3222,7 +3581,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>92</v>
       </c>
@@ -3230,7 +3589,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>100</v>
       </c>
@@ -3238,19 +3597,19 @@
         <v>97641</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1"/>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:25" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" ht="36.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:25" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>457</v>
       </c>
@@ -3327,7 +3686,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -3404,7 +3763,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A13" s="7">
         <v>0.13055555555555556</v>
       </c>
@@ -3481,7 +3840,7 @@
         <v>2.2222222222222223E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>426</v>
       </c>
@@ -3555,7 +3914,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A15" s="6">
         <v>0.19791666666666666</v>
       </c>
@@ -3629,7 +3988,7 @@
         <v>0.13749999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>427</v>
       </c>
@@ -3703,7 +4062,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A17" s="6">
         <v>0.17500000000000002</v>
       </c>
@@ -3777,7 +4136,7 @@
         <v>0.19513888888888889</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>428</v>
       </c>
@@ -3848,7 +4207,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A19" s="6">
         <v>0.15555555555555556</v>
       </c>
@@ -3919,7 +4278,7 @@
         <v>0.20069444444444443</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>429</v>
       </c>
@@ -3990,7 +4349,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A21" s="6">
         <v>7.9861111111111105E-2</v>
       </c>
@@ -4061,7 +4420,7 @@
         <v>0.17013888888888887</v>
       </c>
     </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>430</v>
       </c>
@@ -4132,7 +4491,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A23" s="6">
         <v>8.4722222222222213E-2</v>
       </c>
@@ -4203,7 +4562,7 @@
         <v>0.13472222222222222</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>102</v>
       </c>
@@ -4274,7 +4633,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A25" s="6">
         <v>6.2499999999999995E-3</v>
       </c>
@@ -4345,7 +4704,7 @@
         <v>0.31111111111111112</v>
       </c>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>437</v>
       </c>
@@ -4413,7 +4772,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.45">
       <c r="B27" s="6">
         <v>0.11319444444444444</v>
       </c>
@@ -4481,7 +4840,7 @@
         <v>0.15486111111111112</v>
       </c>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>103</v>
       </c>
@@ -4549,7 +4908,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.45">
       <c r="B29" s="6">
         <v>6.2499999999999995E-3</v>
       </c>
@@ -4617,7 +4976,7 @@
         <v>0.11041666666666666</v>
       </c>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
         <v>438</v>
       </c>
@@ -4685,7 +5044,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
         <v>116</v>
       </c>
@@ -4753,7 +5112,7 @@
         <v>0.36041666666666666</v>
       </c>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
         <v>439</v>
       </c>
@@ -4821,7 +5180,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="33" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B33" s="6">
         <v>7.6388888888888895E-2</v>
       </c>
@@ -4889,7 +5248,7 @@
         <v>5.486111111111111E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
         <v>440</v>
       </c>
@@ -4957,7 +5316,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="35" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B35" s="6">
         <v>0.10833333333333334</v>
       </c>
@@ -5025,7 +5384,7 @@
         <v>0.21180555555555555</v>
       </c>
     </row>
-    <row r="36" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B36" t="s">
         <v>441</v>
       </c>
@@ -5081,7 +5440,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="37" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B37" s="6">
         <v>7.8472222222222221E-2</v>
       </c>
@@ -5137,7 +5496,7 @@
         <v>0.11527777777777777</v>
       </c>
     </row>
-    <row r="38" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B38" t="s">
         <v>442</v>
       </c>
@@ -5190,7 +5549,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="39" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B39" s="6">
         <v>0.14097222222222222</v>
       </c>
@@ -5243,7 +5602,7 @@
         <v>0.38611111111111113</v>
       </c>
     </row>
-    <row r="40" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B40" t="s">
         <v>443</v>
       </c>
@@ -5293,7 +5652,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="41" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B41" s="6">
         <v>8.5416666666666655E-2</v>
       </c>
@@ -5343,7 +5702,7 @@
         <v>4.5138888888888888E-2</v>
       </c>
     </row>
-    <row r="42" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B42" t="s">
         <v>444</v>
       </c>
@@ -5381,7 +5740,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="43" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B43" t="s">
         <v>116</v>
       </c>
@@ -5419,7 +5778,7 @@
         <v>2.0833333333333333E-3</v>
       </c>
     </row>
-    <row r="44" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B44" t="s">
         <v>445</v>
       </c>
@@ -5445,7 +5804,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B45" s="6">
         <v>0.13819444444444443</v>
       </c>
@@ -5471,7 +5830,7 @@
         <v>4.2361111111111106E-2</v>
       </c>
     </row>
-    <row r="46" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B46" t="s">
         <v>446</v>
       </c>
@@ -5494,7 +5853,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B47" s="6">
         <v>7.5694444444444439E-2</v>
       </c>
@@ -5517,7 +5876,7 @@
         <v>4.1666666666666666E-3</v>
       </c>
     </row>
-    <row r="48" spans="2:25" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:25" x14ac:dyDescent="0.45">
       <c r="B48" t="s">
         <v>447</v>
       </c>
@@ -5537,7 +5896,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="49" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B49" s="6">
         <v>0.3972222222222222</v>
       </c>
@@ -5557,7 +5916,7 @@
         <v>0.4284722222222222</v>
       </c>
     </row>
-    <row r="50" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B50" t="s">
         <v>448</v>
       </c>
@@ -5577,7 +5936,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="51" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B51" s="6">
         <v>0.16180555555555556</v>
       </c>
@@ -5597,7 +5956,7 @@
         <v>6.0416666666666667E-2</v>
       </c>
     </row>
-    <row r="52" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B52" t="s">
         <v>449</v>
       </c>
@@ -5617,7 +5976,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="53" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B53" s="6">
         <v>5.9722222222222225E-2</v>
       </c>
@@ -5637,7 +5996,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="54" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B54" t="s">
         <v>450</v>
       </c>
@@ -5657,7 +6016,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="55" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B55" t="s">
         <v>116</v>
       </c>
@@ -5677,7 +6036,7 @@
         <v>6.1805555555555558E-2</v>
       </c>
     </row>
-    <row r="56" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B56" t="s">
         <v>451</v>
       </c>
@@ -5697,7 +6056,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="57" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B57" s="6">
         <v>0.18194444444444444</v>
       </c>
@@ -5717,7 +6076,7 @@
         <v>0.63680555555555551</v>
       </c>
     </row>
-    <row r="58" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B58" t="s">
         <v>452</v>
       </c>
@@ -5734,7 +6093,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="59" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B59" s="6">
         <v>6.5972222222222224E-2</v>
       </c>
@@ -5751,7 +6110,7 @@
         <v>3.7499999999999999E-2</v>
       </c>
     </row>
-    <row r="60" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B60" t="s">
         <v>453</v>
       </c>
@@ -5768,7 +6127,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="61" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B61" s="6">
         <v>0.14375000000000002</v>
       </c>
@@ -5785,7 +6144,7 @@
         <v>0.24583333333333335</v>
       </c>
     </row>
-    <row r="62" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B62" t="s">
         <v>454</v>
       </c>
@@ -5802,7 +6161,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="63" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B63" s="6">
         <v>0.13541666666666666</v>
       </c>
@@ -5819,7 +6178,7 @@
         <v>4.7222222222222221E-2</v>
       </c>
     </row>
-    <row r="64" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B64" t="s">
         <v>455</v>
       </c>
@@ -5833,7 +6192,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="65" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B65" s="6">
         <v>5.1388888888888894E-2</v>
       </c>
@@ -5847,7 +6206,7 @@
         <v>0.34166666666666662</v>
       </c>
     </row>
-    <row r="66" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B66" t="s">
         <v>456</v>
       </c>
@@ -5858,7 +6217,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="67" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B67" t="s">
         <v>116</v>
       </c>
@@ -5869,22 +6228,22 @@
         <v>3.472222222222222E-3</v>
       </c>
     </row>
-    <row r="68" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B68" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="69" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B69" s="6">
         <v>3.0555555555555555E-2</v>
       </c>
     </row>
-    <row r="70" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B70" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="71" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:21" x14ac:dyDescent="0.45">
       <c r="B71" s="6">
         <v>1.5972222222222224E-2</v>
       </c>
@@ -5895,29 +6254,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="38.125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="38.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="30.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.1328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="48.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="52.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="48.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.265625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="44" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="38.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="38.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="38.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>84</v>
       </c>
@@ -5925,7 +6284,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>86</v>
       </c>
@@ -5933,7 +6292,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>88</v>
       </c>
@@ -5941,7 +6300,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>97</v>
       </c>
@@ -5949,7 +6308,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>90</v>
       </c>
@@ -5957,7 +6316,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>92</v>
       </c>
@@ -5965,7 +6324,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>100</v>
       </c>
@@ -5973,19 +6332,19 @@
         <v>8124</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1"/>
       <c r="B8" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:10" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>482</v>
       </c>
@@ -6017,7 +6376,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -6046,7 +6405,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="6">
         <v>0.11527777777777777</v>
       </c>
@@ -6078,7 +6437,7 @@
         <v>0.17222222222222225</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>498</v>
       </c>
@@ -6110,7 +6469,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="6">
         <v>4.1666666666666664E-2</v>
       </c>
@@ -6142,7 +6501,7 @@
         <v>0.26319444444444445</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>499</v>
       </c>
@@ -6174,7 +6533,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="6">
         <v>0.14166666666666666</v>
       </c>
@@ -6206,7 +6565,7 @@
         <v>0.1125</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>503</v>
       </c>
@@ -6235,7 +6594,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B19" s="6">
         <v>0.26527777777777778</v>
       </c>
@@ -6264,7 +6623,7 @@
         <v>0.2638888888888889</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>504</v>
       </c>
@@ -6287,7 +6646,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B21" s="6">
         <v>0.26250000000000001</v>
       </c>
@@ -6310,7 +6669,7 @@
         <v>0.20138888888888887</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
         <v>505</v>
       </c>
@@ -6333,7 +6692,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B23" s="6">
         <v>0.24444444444444446</v>
       </c>
@@ -6356,7 +6715,7 @@
         <v>0.2388888888888889</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
         <v>506</v>
       </c>
@@ -6379,7 +6738,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B25" s="6">
         <v>0.24305555555555555</v>
       </c>
@@ -6402,7 +6761,7 @@
         <v>0.37013888888888885</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>507</v>
       </c>
@@ -6425,7 +6784,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B27" s="6">
         <v>0.19722222222222222</v>
       </c>
@@ -6448,7 +6807,7 @@
         <v>0.31736111111111115</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>508</v>
       </c>
@@ -6471,7 +6830,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B29" s="6">
         <v>0.13263888888888889</v>
       </c>
@@ -6494,7 +6853,7 @@
         <v>0.18263888888888891</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
         <v>509</v>
       </c>
@@ -6514,7 +6873,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B31" s="6">
         <v>0.21666666666666667</v>
       </c>
@@ -6534,7 +6893,7 @@
         <v>0.21527777777777779</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
         <v>510</v>
       </c>
@@ -6554,7 +6913,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B33" s="6">
         <v>0.32847222222222222</v>
       </c>
@@ -6574,7 +6933,7 @@
         <v>0.19930555555555554</v>
       </c>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
         <v>511</v>
       </c>
@@ -6591,7 +6950,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.45">
       <c r="B35" s="6">
         <v>0.32708333333333334</v>
       </c>
@@ -6608,7 +6967,7 @@
         <v>6.8749999999999992E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.45">
       <c r="E36" s="6">
         <v>0.47847222222222219</v>
       </c>
@@ -6619,7 +6978,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.45">
       <c r="E37" t="s">
         <v>543</v>
       </c>
@@ -6630,7 +6989,7 @@
         <v>0.3430555555555555</v>
       </c>
     </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.45">
       <c r="E38" s="6">
         <v>0.4145833333333333</v>
       </c>
@@ -6641,7 +7000,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:10" x14ac:dyDescent="0.45">
       <c r="E39" t="s">
         <v>544</v>
       </c>
@@ -6652,7 +7011,7 @@
         <v>0.20138888888888887</v>
       </c>
     </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:10" x14ac:dyDescent="0.45">
       <c r="E40" s="6">
         <v>0.18472222222222223</v>
       </c>
@@ -6660,7 +7019,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.45">
       <c r="E41" t="s">
         <v>545</v>
       </c>
@@ -6668,7 +7027,7 @@
         <v>0.3215277777777778</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.45">
       <c r="E42" s="6">
         <v>0.37708333333333338</v>
       </c>
@@ -6676,7 +7035,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.45">
       <c r="E43" t="s">
         <v>546</v>
       </c>
@@ -6684,7 +7043,7 @@
         <v>0.2951388888888889</v>
       </c>
     </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.45">
       <c r="E44" s="6">
         <v>0.21388888888888891</v>
       </c>
@@ -6692,7 +7051,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.45">
       <c r="E45" t="s">
         <v>547</v>
       </c>
@@ -6700,7 +7059,7 @@
         <v>0.37291666666666662</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:10" x14ac:dyDescent="0.45">
       <c r="E46" s="6">
         <v>0.34722222222222227</v>
       </c>
@@ -6708,7 +7067,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.45">
       <c r="E47" t="s">
         <v>548</v>
       </c>
@@ -6716,7 +7075,7 @@
         <v>0.35000000000000003</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.45">
       <c r="E48" s="6">
         <v>0.3972222222222222</v>
       </c>
@@ -6724,7 +7083,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="49" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="5:7" x14ac:dyDescent="0.45">
       <c r="E49" t="s">
         <v>549</v>
       </c>
@@ -6732,7 +7091,7 @@
         <v>0.33055555555555555</v>
       </c>
     </row>
-    <row r="50" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="5:7" x14ac:dyDescent="0.45">
       <c r="E50" s="6">
         <v>0.27916666666666667</v>
       </c>
@@ -6740,7 +7099,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="51" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="5:7" x14ac:dyDescent="0.45">
       <c r="E51" t="s">
         <v>550</v>
       </c>
@@ -6748,7 +7107,7 @@
         <v>0.29652777777777778</v>
       </c>
     </row>
-    <row r="52" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="5:7" x14ac:dyDescent="0.45">
       <c r="E52" s="6">
         <v>0.28611111111111115</v>
       </c>
@@ -6756,7 +7115,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="53" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="5:7" x14ac:dyDescent="0.45">
       <c r="E53" t="s">
         <v>551</v>
       </c>
@@ -6764,7 +7123,7 @@
         <v>0.27916666666666667</v>
       </c>
     </row>
-    <row r="54" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="5:7" x14ac:dyDescent="0.45">
       <c r="E54" s="6">
         <v>0.35347222222222219</v>
       </c>
@@ -6772,7 +7131,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="55" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="5:7" x14ac:dyDescent="0.45">
       <c r="E55" t="s">
         <v>552</v>
       </c>
@@ -6780,7 +7139,7 @@
         <v>0.35694444444444445</v>
       </c>
     </row>
-    <row r="56" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="5:7" x14ac:dyDescent="0.45">
       <c r="E56" s="6">
         <v>5.8333333333333327E-2</v>
       </c>
@@ -6788,47 +7147,47 @@
         <v>586</v>
       </c>
     </row>
-    <row r="57" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="5:7" x14ac:dyDescent="0.45">
       <c r="G57" s="6">
         <v>0.1013888888888889</v>
       </c>
     </row>
-    <row r="58" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="5:7" x14ac:dyDescent="0.45">
       <c r="G58" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="59" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="5:7" x14ac:dyDescent="0.45">
       <c r="G59" s="6">
         <v>0.40486111111111112</v>
       </c>
     </row>
-    <row r="60" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="5:7" x14ac:dyDescent="0.45">
       <c r="G60" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="61" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="5:7" x14ac:dyDescent="0.45">
       <c r="G61" s="6">
         <v>0.37916666666666665</v>
       </c>
     </row>
-    <row r="62" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="5:7" x14ac:dyDescent="0.45">
       <c r="G62" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="63" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="5:7" x14ac:dyDescent="0.45">
       <c r="G63" s="6">
         <v>0.16527777777777777</v>
       </c>
     </row>
-    <row r="64" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="5:7" x14ac:dyDescent="0.45">
       <c r="G64" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="65" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="7:7" x14ac:dyDescent="0.45">
       <c r="G65" s="6">
         <v>0.1451388888888889</v>
       </c>

</xml_diff>